<commit_message>
Tp3 .fst files and correction in Tp2
</commit_message>
<xml_diff>
--- a/01_Simulations/01_Sim/SimOneSeed/Parametermatrix.xlsx
+++ b/01_Simulations/01_Sim/SimOneSeed/Parametermatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tp1-Curve" sheetId="3" r:id="rId1"/>
@@ -1900,6 +1900,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1930,15 +1948,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1959,15 +1968,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2032,7 +2032,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2153,6 +2152,493 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6493-40BB-AEA0-67FF42C75991}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="457073576"/>
+        <c:axId val="457072264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="457073576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Significant wave heigth (m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-DE" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457072264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="457072264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1400"/>
+                  <a:t>Spectral peak period (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="457073576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>=WURZEL((2*PI()*hs)/(9.81*(1/20)))</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Tp2-Curve'!$C$27:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Tp2-Curve'!$D$27:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.5790719436664071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1991344503745109</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0030481624003844</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.4693342873498896</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.737215830999221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.87043873482949</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.904527411463793</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.861686032698204</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0622-4B7F-A16F-8CDEE76A10E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2366,492 +2852,6 @@
             </c:rich>
           </c:tx>
           <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="457073576"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>=WURZEL((2*PI()*hs)/(9.81*(1/20)))</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Tp2-Curve'!$C$27:$C$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>15</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Tp2-Curve'!$D$27:$D$34</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3.5790719436664071</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.1991344503745109</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.0030481624003844</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9.4693342873498896</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.737215830999221</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.87043873482949</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>12.904527411463793</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>13.861686032698204</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0622-4B7F-A16F-8CDEE76A10E0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="457073576"/>
-        <c:axId val="457072264"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="457073576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:sysClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE" sz="1400" b="0" i="0" baseline="0">
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Significant wave heigth (m)</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE" sz="1400">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                <a:lnSpc>
-                  <a:spcPct val="100000"/>
-                </a:lnSpc>
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-                <a:buClrTx/>
-                <a:buSzTx/>
-                <a:buFontTx/>
-                <a:buNone/>
-                <a:tabLst/>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:sysClr val="windowText" lastClr="000000">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:sysClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="457072264"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="457072264"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE" sz="1400"/>
-                  <a:t>Spectral peak period (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6594,46 +6594,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="66"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="49"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="57" t="s">
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="59"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="62"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="27">
         <v>1</v>
       </c>
@@ -6675,7 +6675,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -6723,12 +6723,12 @@
       <c r="P4" s="14">
         <v>3.0995672251872559</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -6774,10 +6774,10 @@
       <c r="P5" s="20">
         <v>5.3686079154996103</v>
       </c>
-      <c r="Q5" s="55"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -6823,10 +6823,10 @@
       <c r="P6" s="20">
         <v>6.9308430163491019</v>
       </c>
-      <c r="Q6" s="55"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="15">
         <v>7</v>
       </c>
@@ -6872,10 +6872,10 @@
       <c r="P7" s="20">
         <v>8.2006840497720184</v>
       </c>
-      <c r="Q7" s="55"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="15">
         <v>9</v>
       </c>
@@ -6921,10 +6921,10 @@
       <c r="P8" s="20">
         <v>9.2987016755617677</v>
       </c>
-      <c r="Q8" s="55"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="15">
         <v>11</v>
       </c>
@@ -6970,10 +6970,10 @@
       <c r="P9" s="20">
         <v>10.280101498429151</v>
       </c>
-      <c r="Q9" s="55"/>
+      <c r="Q9" s="45"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="21">
         <v>13</v>
       </c>
@@ -7019,10 +7019,10 @@
       <c r="P10" s="26">
         <v>11.175648562160289</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="45"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="2">
         <v>15</v>
       </c>
@@ -7068,30 +7068,30 @@
       <c r="P11" s="3">
         <v>12.004572243600576</v>
       </c>
-      <c r="Q11" s="56"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="48" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -7101,8 +7101,8 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="5">
         <v>26</v>
       </c>
@@ -7127,7 +7127,7 @@
       <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="9">
@@ -7151,7 +7151,7 @@
       <c r="H16" s="28">
         <v>3.0995672251872559</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="44" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="33"/>
@@ -7164,7 +7164,7 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="15">
         <v>3</v>
       </c>
@@ -7186,7 +7186,7 @@
       <c r="H17" s="29">
         <v>5.3686079154996103</v>
       </c>
-      <c r="I17" s="55"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
@@ -7197,7 +7197,7 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="15">
         <v>5</v>
       </c>
@@ -7219,7 +7219,7 @@
       <c r="H18" s="29">
         <v>6.9308430163491019</v>
       </c>
-      <c r="I18" s="55"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
@@ -7230,7 +7230,7 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="15">
         <v>7</v>
       </c>
@@ -7252,7 +7252,7 @@
       <c r="H19" s="29">
         <v>8.2006840497720184</v>
       </c>
-      <c r="I19" s="55"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -7263,7 +7263,7 @@
       <c r="Q19" s="33"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="15">
         <v>9</v>
       </c>
@@ -7285,7 +7285,7 @@
       <c r="H20" s="29">
         <v>9.2987016755617677</v>
       </c>
-      <c r="I20" s="55"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
@@ -7296,7 +7296,7 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="15">
         <v>11</v>
       </c>
@@ -7318,7 +7318,7 @@
       <c r="H21" s="29">
         <v>10.280101498429151</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="33"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -7329,7 +7329,7 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="21">
         <v>13</v>
       </c>
@@ -7351,7 +7351,7 @@
       <c r="H22" s="30">
         <v>11.175648562160289</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -7362,7 +7362,7 @@
       <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="2">
         <v>15</v>
       </c>
@@ -7384,7 +7384,7 @@
       <c r="H23" s="31">
         <v>12.004572243600576</v>
       </c>
-      <c r="I23" s="56"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
@@ -7483,16 +7483,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="I16:I23"/>
+    <mergeCell ref="C2:O2"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="Q4:Q11"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="I16:I23"/>
-    <mergeCell ref="C2:O2"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7504,7 +7504,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D34"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7515,48 +7515,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="67"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="50"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="43">
         <v>1</v>
       </c>
@@ -7599,7 +7599,7 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -7647,12 +7647,12 @@
       <c r="P4" s="14">
         <v>3.5790719436664071</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -7698,10 +7698,10 @@
       <c r="P5" s="20">
         <v>6.1991344503745109</v>
       </c>
-      <c r="Q5" s="55"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -7747,10 +7747,10 @@
       <c r="P6" s="20">
         <v>8.0030481624003844</v>
       </c>
-      <c r="Q6" s="55"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="15">
         <v>7</v>
       </c>
@@ -7796,10 +7796,10 @@
       <c r="P7" s="20">
         <v>9.4693342873498896</v>
       </c>
-      <c r="Q7" s="55"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="15">
         <v>9</v>
       </c>
@@ -7843,10 +7843,10 @@
       <c r="P8" s="20">
         <v>10.737215830999221</v>
       </c>
-      <c r="Q8" s="55"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="15">
         <v>11</v>
       </c>
@@ -7890,10 +7890,10 @@
       <c r="P9" s="20">
         <v>11.87043873482949</v>
       </c>
-      <c r="Q9" s="55"/>
+      <c r="Q9" s="45"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="21">
         <v>13</v>
       </c>
@@ -7937,10 +7937,10 @@
       <c r="P10" s="26">
         <v>12.904527411463793</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="45"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="2">
         <v>15</v>
       </c>
@@ -7984,32 +7984,32 @@
       <c r="P11" s="3">
         <v>13.861686032698204</v>
       </c>
-      <c r="Q11" s="56"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -8019,8 +8019,8 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="5">
         <v>26</v>
       </c>
@@ -8045,7 +8045,7 @@
       <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="9">
@@ -8069,7 +8069,7 @@
       <c r="H16" s="28">
         <v>3.5790719436664071</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="44" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="33"/>
@@ -8082,7 +8082,7 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="15">
         <v>3</v>
       </c>
@@ -8104,7 +8104,7 @@
       <c r="H17" s="29">
         <v>6.1991344503745109</v>
       </c>
-      <c r="I17" s="55"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
@@ -8115,7 +8115,7 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="15">
         <v>5</v>
       </c>
@@ -8137,7 +8137,7 @@
       <c r="H18" s="29">
         <v>8.0030481624003844</v>
       </c>
-      <c r="I18" s="55"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
@@ -8148,7 +8148,7 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="15">
         <v>7</v>
       </c>
@@ -8170,7 +8170,7 @@
       <c r="H19" s="29">
         <v>9.4693342873498896</v>
       </c>
-      <c r="I19" s="55"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -8181,7 +8181,7 @@
       <c r="Q19" s="33"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="15">
         <v>9</v>
       </c>
@@ -8203,7 +8203,7 @@
       <c r="H20" s="29">
         <v>10.737215830999221</v>
       </c>
-      <c r="I20" s="55"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
@@ -8214,7 +8214,7 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="15">
         <v>11</v>
       </c>
@@ -8236,7 +8236,7 @@
       <c r="H21" s="29">
         <v>11.87043873482949</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="33"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -8247,7 +8247,7 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="21">
         <v>13</v>
       </c>
@@ -8269,7 +8269,7 @@
       <c r="H22" s="30">
         <v>12.904527411463793</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -8280,7 +8280,7 @@
       <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="2">
         <v>15</v>
       </c>
@@ -8302,7 +8302,7 @@
       <c r="H23" s="31">
         <v>13.861686032698204</v>
       </c>
-      <c r="I23" s="56"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
@@ -8416,16 +8416,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="I16:I23"/>
+    <mergeCell ref="C2:P2"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="Q4:Q11"/>
     <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A14:B15"/>
-    <mergeCell ref="C14:G14"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="I16:I23"/>
-    <mergeCell ref="C2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8436,7 +8436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -8448,48 +8448,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="67"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="50"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="43">
         <v>1</v>
       </c>
@@ -8532,7 +8532,7 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -8580,12 +8580,12 @@
       <c r="P4" s="14">
         <v>6.5072751739419168</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -8631,10 +8631,10 @@
       <c r="P5" s="20">
         <v>8.6712704053740897</v>
       </c>
-      <c r="Q5" s="55"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -8680,10 +8680,10 @@
       <c r="P6" s="20">
         <v>10.1973832438198</v>
       </c>
-      <c r="Q6" s="55"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="15">
         <v>7</v>
       </c>
@@ -8729,10 +8729,10 @@
       <c r="P7" s="20">
         <v>11.46933428734989</v>
       </c>
-      <c r="Q7" s="55"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="15">
         <v>9</v>
       </c>
@@ -8776,10 +8776,10 @@
       <c r="P8" s="20">
         <v>12.59051566328354</v>
       </c>
-      <c r="Q8" s="55"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="15">
         <v>11</v>
       </c>
@@ -8823,10 +8823,10 @@
       <c r="P9" s="20">
         <v>13.607472918472149</v>
       </c>
-      <c r="Q9" s="55"/>
+      <c r="Q9" s="45"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="21">
         <v>13</v>
       </c>
@@ -8870,10 +8870,10 @@
       <c r="P10" s="26">
         <v>14.546232180725173</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="45"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="2">
         <v>15</v>
       </c>
@@ -8917,32 +8917,32 @@
       <c r="P11" s="3">
         <v>15.423238845507035</v>
       </c>
-      <c r="Q11" s="56"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -8952,8 +8952,8 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="5">
         <v>26</v>
       </c>
@@ -8978,7 +8978,7 @@
       <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="9">
@@ -9002,7 +9002,7 @@
       <c r="H16" s="28">
         <v>6.5072751739419168</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="44" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="33"/>
@@ -9015,7 +9015,7 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="15">
         <v>3</v>
       </c>
@@ -9037,7 +9037,7 @@
       <c r="H17" s="29">
         <v>8.6712704053740897</v>
       </c>
-      <c r="I17" s="55"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
@@ -9048,7 +9048,7 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="15">
         <v>5</v>
       </c>
@@ -9070,7 +9070,7 @@
       <c r="H18" s="29">
         <v>10.197383243819839</v>
       </c>
-      <c r="I18" s="55"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
@@ -9081,7 +9081,7 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="15">
         <v>7</v>
       </c>
@@ -9103,7 +9103,7 @@
       <c r="H19" s="29">
         <v>11.46933428734989</v>
       </c>
-      <c r="I19" s="55"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -9114,7 +9114,7 @@
       <c r="Q19" s="33"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="15">
         <v>9</v>
       </c>
@@ -9136,7 +9136,7 @@
       <c r="H20" s="29">
         <v>12.59051566328354</v>
       </c>
-      <c r="I20" s="55"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
@@ -9147,7 +9147,7 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="15">
         <v>11</v>
       </c>
@@ -9169,7 +9169,7 @@
       <c r="H21" s="29">
         <v>13.607472918472149</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="33"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -9180,7 +9180,7 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="21">
         <v>13</v>
       </c>
@@ -9202,7 +9202,7 @@
       <c r="H22" s="30">
         <v>14.546232180725173</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -9213,7 +9213,7 @@
       <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="2">
         <v>15</v>
       </c>
@@ -9235,7 +9235,7 @@
       <c r="H23" s="31">
         <v>15.423238845507035</v>
       </c>
-      <c r="I23" s="56"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
@@ -9349,16 +9349,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="Q4:Q11"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="A16:A23"/>
     <mergeCell ref="I16:I23"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9369,7 +9369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K20" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -9381,48 +9381,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="49"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="67"/>
       <c r="B2" s="68"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="50"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="56"/>
     </row>
     <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="43">
         <v>1</v>
       </c>
@@ -9465,7 +9465,7 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9">
@@ -9513,12 +9513,12 @@
       <c r="P4" s="14">
         <v>10.899580019355181</v>
       </c>
-      <c r="Q4" s="54" t="s">
+      <c r="Q4" s="44" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="52"/>
+      <c r="A5" s="58"/>
       <c r="B5" s="15">
         <v>3</v>
       </c>
@@ -9564,10 +9564,10 @@
       <c r="P5" s="20">
         <v>12.379474337873459</v>
       </c>
-      <c r="Q5" s="55"/>
+      <c r="Q5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="52"/>
+      <c r="A6" s="58"/>
       <c r="B6" s="15">
         <v>5</v>
       </c>
@@ -9613,10 +9613,10 @@
       <c r="P6" s="20">
         <v>13.488885865949019</v>
       </c>
-      <c r="Q6" s="55"/>
+      <c r="Q6" s="45"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
+      <c r="A7" s="58"/>
       <c r="B7" s="15">
         <v>7</v>
       </c>
@@ -9662,10 +9662,10 @@
       <c r="P7" s="20">
         <v>14.46933428734989</v>
       </c>
-      <c r="Q7" s="55"/>
+      <c r="Q7" s="45"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
+      <c r="A8" s="58"/>
       <c r="B8" s="15">
         <v>9</v>
       </c>
@@ -9709,10 +9709,10 @@
       <c r="P8" s="20">
         <v>15.37046541171002</v>
       </c>
-      <c r="Q8" s="55"/>
+      <c r="Q8" s="45"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
+      <c r="A9" s="58"/>
       <c r="B9" s="15">
         <v>11</v>
       </c>
@@ -9756,10 +9756,10 @@
       <c r="P9" s="20">
         <v>16.213024193936139</v>
       </c>
-      <c r="Q9" s="55"/>
+      <c r="Q9" s="45"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
+      <c r="A10" s="58"/>
       <c r="B10" s="21">
         <v>13</v>
       </c>
@@ -9803,10 +9803,10 @@
       <c r="P10" s="26">
         <v>17.008789334617244</v>
       </c>
-      <c r="Q10" s="55"/>
+      <c r="Q10" s="45"/>
     </row>
     <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="53"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="2">
         <v>15</v>
       </c>
@@ -9850,32 +9850,32 @@
       <c r="P11" s="3">
         <v>17.765568064720281</v>
       </c>
-      <c r="Q11" s="56"/>
+      <c r="Q11" s="46"/>
     </row>
     <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="64" t="s">
+      <c r="A13" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="51"/>
+      <c r="C14" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -9885,8 +9885,8 @@
       <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
       <c r="C15" s="5">
         <v>26</v>
       </c>
@@ -9911,7 +9911,7 @@
       <c r="N15" s="33"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="57" t="s">
         <v>3</v>
       </c>
       <c r="B16" s="9">
@@ -9935,7 +9935,7 @@
       <c r="H16" s="28">
         <v>10.899580019355181</v>
       </c>
-      <c r="I16" s="54" t="s">
+      <c r="I16" s="44" t="s">
         <v>4</v>
       </c>
       <c r="J16" s="33"/>
@@ -9948,7 +9948,7 @@
       <c r="Q16" s="33"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="52"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="15">
         <v>3</v>
       </c>
@@ -9970,7 +9970,7 @@
       <c r="H17" s="29">
         <v>12.379474337873459</v>
       </c>
-      <c r="I17" s="55"/>
+      <c r="I17" s="45"/>
       <c r="J17" s="33"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
@@ -9981,7 +9981,7 @@
       <c r="Q17" s="33"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="52"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="15">
         <v>5</v>
       </c>
@@ -10003,7 +10003,7 @@
       <c r="H18" s="29">
         <v>13.488885865949019</v>
       </c>
-      <c r="I18" s="55"/>
+      <c r="I18" s="45"/>
       <c r="J18" s="33"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
@@ -10014,7 +10014,7 @@
       <c r="Q18" s="33"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="15">
         <v>7</v>
       </c>
@@ -10036,7 +10036,7 @@
       <c r="H19" s="29">
         <v>14.46933428734989</v>
       </c>
-      <c r="I19" s="55"/>
+      <c r="I19" s="45"/>
       <c r="J19" s="33"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
@@ -10047,7 +10047,7 @@
       <c r="Q19" s="33"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="15">
         <v>9</v>
       </c>
@@ -10069,7 +10069,7 @@
       <c r="H20" s="29">
         <v>15.37046541171002</v>
       </c>
-      <c r="I20" s="55"/>
+      <c r="I20" s="45"/>
       <c r="J20" s="33"/>
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
@@ -10080,7 +10080,7 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="15">
         <v>11</v>
       </c>
@@ -10102,7 +10102,7 @@
       <c r="H21" s="29">
         <v>16.213024193936139</v>
       </c>
-      <c r="I21" s="55"/>
+      <c r="I21" s="45"/>
       <c r="J21" s="33"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
@@ -10113,7 +10113,7 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="21">
         <v>13</v>
       </c>
@@ -10135,7 +10135,7 @@
       <c r="H22" s="30">
         <v>17.008789334617244</v>
       </c>
-      <c r="I22" s="55"/>
+      <c r="I22" s="45"/>
       <c r="J22" s="33"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
@@ -10146,7 +10146,7 @@
       <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="53"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="2">
         <v>15</v>
       </c>
@@ -10168,7 +10168,7 @@
       <c r="H23" s="31">
         <v>17.765568064720281</v>
       </c>
-      <c r="I23" s="56"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
@@ -10282,16 +10282,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="C2:P2"/>
+    <mergeCell ref="A4:A11"/>
     <mergeCell ref="Q4:Q11"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:G14"/>
     <mergeCell ref="A16:A23"/>
     <mergeCell ref="I16:I23"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="C2:P2"/>
-    <mergeCell ref="A4:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>